<commit_message>
Entrega RF0003 y RF0004
</commit_message>
<xml_diff>
--- a/SIGOFCv3/Archivos/Plantilla/InformeFaunaInfraestructura.xlsx
+++ b/SIGOFCv3/Archivos/Plantilla/InformeFaunaInfraestructura.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioSIGO\SIGOsfc\SIGOFCv3\Archivos\Plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\Repos_Azure_Osinfor\SIGOsfc\SIGOFCv3\Archivos\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC40F55D-2C51-465B-83BD-8F09419E7115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="10560"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>INFRAESTRUCTURA_MATERIAL</t>
   </si>
@@ -355,12 +356,18 @@
   </si>
   <si>
     <t>TECHO DE TEJA</t>
+  </si>
+  <si>
+    <t>COORDENADA_ESTE</t>
+  </si>
+  <si>
+    <t>COORDENADA_NORTE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -516,6 +523,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -551,6 +575,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -726,11 +767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,24 +781,26 @@
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="7" width="28.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1"/>
-    <col min="14" max="14" width="26.42578125" customWidth="1"/>
-    <col min="15" max="15" width="29" customWidth="1"/>
-    <col min="16" max="16" width="27" customWidth="1"/>
-    <col min="17" max="17" width="26" customWidth="1"/>
-    <col min="18" max="18" width="29.140625" customWidth="1"/>
-    <col min="19" max="19" width="31.42578125" customWidth="1"/>
-    <col min="20" max="20" width="35" customWidth="1"/>
-    <col min="21" max="21" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="9" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" customWidth="1"/>
+    <col min="17" max="17" width="29" customWidth="1"/>
+    <col min="18" max="18" width="27" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="20" max="20" width="29.140625" customWidth="1"/>
+    <col min="21" max="21" width="31.42578125" customWidth="1"/>
+    <col min="22" max="22" width="35" customWidth="1"/>
+    <col min="23" max="23" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -774,57 +817,63 @@
         <v>62</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:O1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INFRAESTRUCTURA_CARTEL</formula1>
     </dataValidation>
   </dataValidations>
@@ -832,17 +881,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Hoja1!$E$2:$E$51</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:U1048576</xm:sqref>
+          <xm:sqref>P2:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Hoja1!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:J1048576</xm:sqref>
+          <xm:sqref>H2:L1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -851,7 +900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">

</xml_diff>